<commit_message>
Vorstellung Arch + Erklärung
</commit_message>
<xml_diff>
--- a/Sonstiges/MFEM-Beispiel-Spring.xlsx
+++ b/Sonstiges/MFEM-Beispiel-Spring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="QUT-GQM" sheetId="2" r:id="rId1"/>
@@ -838,6 +838,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -849,23 +855,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1064,11 +1064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066138656"/>
-        <c:axId val="2066140432"/>
+        <c:axId val="176128320"/>
+        <c:axId val="215946448"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2066138656"/>
+        <c:axId val="176128320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2066140432"/>
+        <c:crossAx val="215946448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1119,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066140432"/>
+        <c:axId val="215946448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1170,7 +1170,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2066138656"/>
+        <c:crossAx val="176128320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2064,13 +2064,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="22" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" style="39" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" style="22" customWidth="1"/>
@@ -2111,7 +2111,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="20">
@@ -2141,11 +2141,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
-      <c r="B3" s="50">
+      <c r="A3" s="49"/>
+      <c r="B3" s="52">
         <v>2</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="50" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="20">
@@ -2169,9 +2169,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="21">
         <v>3</v>
       </c>
@@ -2193,11 +2193,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57"/>
-      <c r="B5" s="50">
+      <c r="A5" s="54"/>
+      <c r="B5" s="52">
         <v>3</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="20">
@@ -2221,9 +2221,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="20">
         <v>5</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="21">
         <v>4</v>
       </c>
@@ -2273,7 +2273,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="43">
@@ -2303,7 +2303,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="20">
         <v>6</v>
       </c>
@@ -2331,7 +2331,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="21">
         <v>7</v>
       </c>
@@ -2359,13 +2359,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="52">
         <v>8</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="50" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="21">
@@ -2389,9 +2389,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="49"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="20">
         <v>11</v>
       </c>
@@ -2413,17 +2413,17 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-      <c r="B13" s="50">
+      <c r="A13" s="55"/>
+      <c r="B13" s="52">
         <v>9</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="52">
         <v>12</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="50" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="36">
@@ -2441,11 +2441,11 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="49"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="36">
         <v>13</v>
       </c>
@@ -2461,9 +2461,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="20">
         <v>13</v>
       </c>
@@ -2485,9 +2485,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="20">
         <v>14</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="21">
         <v>10</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="48" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="21">
@@ -2567,7 +2567,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="20">
         <v>12</v>
       </c>
@@ -2595,13 +2595,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="52">
         <v>13</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="50" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="21">
@@ -2625,9 +2625,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="49"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="20">
         <v>19</v>
       </c>
@@ -2649,11 +2649,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="53"/>
-      <c r="B22" s="50">
+      <c r="A22" s="55"/>
+      <c r="B22" s="52">
         <v>14</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="50" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="20">
@@ -2677,9 +2677,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="49"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="20">
         <v>21</v>
       </c>
@@ -2701,13 +2701,13 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="50">
+      <c r="B24" s="52">
         <v>15</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="50" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="21">
@@ -2731,13 +2731,13 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="53"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="50">
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="52">
         <v>23</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="50" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="36">
@@ -2755,11 +2755,11 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="53"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="36">
         <v>25</v>
       </c>
@@ -2775,9 +2775,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="21">
         <v>24</v>
       </c>
@@ -3024,6 +3024,20 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
@@ -3034,20 +3048,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>